<commit_message>
update W6D1 Pandas notebook
</commit_message>
<xml_diff>
--- a/data/new.xlsx
+++ b/data/new.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khueluu/Desktop/NSU/Teaching/Python/NSU_Python/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31E2E45-1A87-7545-AB81-F2FFFF1404FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -37,8 +31,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,14 +95,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -155,7 +141,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,27 +173,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,24 +207,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -432,16 +382,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -472,7 +420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -489,7 +437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -502,8 +450,11 @@
       <c r="D4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -517,7 +468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -530,11 +481,8 @@
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>

</xml_diff>